<commit_message>
Complete Warehouse System with User Interface
</commit_message>
<xml_diff>
--- a/Warehouse-System/Prices.xlsx
+++ b/Warehouse-System/Prices.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Commodity</t>
   </si>
@@ -29,6 +29,12 @@
   </si>
   <si>
     <t>Cashewnuts</t>
+  </si>
+  <si>
+    <t>Coconut</t>
+  </si>
+  <si>
+    <t>Black pepper</t>
   </si>
 </sst>
 </file>
@@ -386,7 +392,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -424,6 +430,22 @@
         <v>13500</v>
       </c>
     </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>22500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>36000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>